<commit_message>
Included exgtra item on BOM and initial presentation file
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Item Description</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/Adhere-Fly-Aluminum-Thermostat-Temperature/dp/B01N0Q9RQ4/ref=pd_day0_107_9?_encoding=UTF8&amp;psc=1&amp;refRID=QCTZEQQF5RFKNGRZ3H98</t>
+  </si>
+  <si>
+    <t>B01N0Q9RQ4</t>
+  </si>
+  <si>
+    <t>12V 150W Heater </t>
+  </si>
+  <si>
+    <t>Adhere To Fly</t>
   </si>
 </sst>
 </file>
@@ -441,7 +453,7 @@
   <dimension ref="A1:I200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,9 +589,24 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="2"/>
+      <c r="B10" s="5">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
@@ -595,8 +622,8 @@
         <v>27</v>
       </c>
       <c r="B13" s="5">
-        <f>SUM(B6:B9)</f>
-        <v>44.5</v>
+        <f>SUM(B6:B10)</f>
+        <v>51.5</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="2"/>

</xml_diff>

<commit_message>
Included relay module in BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Item Description</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>Adhere To Fly</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/Demarkt-Channel-Optocoupler-Isolation-Support/dp/B06Y5GRC4P/ref=sr_1_1?s=kitchen&amp;ie=UTF8&amp;qid=1517403224&amp;sr=8-1&amp;keywords=B06Y5GRC4P</t>
+  </si>
+  <si>
+    <t>B06Y5GRC4P</t>
+  </si>
+  <si>
+    <t>Demarkt</t>
+  </si>
+  <si>
+    <t>Relay Module</t>
   </si>
 </sst>
 </file>
@@ -450,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I200"/>
+  <dimension ref="A1:I201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,6 +515,9 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
       <c r="B6" s="5">
         <v>17.5</v>
       </c>
@@ -526,8 +541,11 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
       <c r="B7" s="5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -549,6 +567,9 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
       <c r="B8" s="5">
         <v>11</v>
       </c>
@@ -569,6 +590,9 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
       <c r="B9" s="5">
         <v>8</v>
       </c>
@@ -589,6 +613,9 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
       <c r="B10" s="5">
         <v>7</v>
       </c>
@@ -609,26 +636,45 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="2"/>
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
       <c r="H12" s="4"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="5">
-        <f>SUM(B6:B10)</f>
-        <v>51.5</v>
-      </c>
       <c r="H13" s="4"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="5">
+        <f>SUM(B6:B11)</f>
+        <v>48.5</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="2"/>
     </row>
@@ -685,6 +731,7 @@
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H28" s="4"/>
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="8:9" x14ac:dyDescent="0.25">
@@ -1202,6 +1249,9 @@
     </row>
     <row r="200" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I200" s="2"/>
+    </row>
+    <row r="201" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I201" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Included power board design and renamed circuit design files directory
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17760" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
   <si>
     <t>Item Description</t>
   </si>
@@ -139,16 +139,175 @@
   </si>
   <si>
     <t>Plug Adapter</t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>Digi-key</t>
+  </si>
+  <si>
+    <t>WM3843-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/product-detail/en/molex-llc/0039293026/WM3843-ND/2002650</t>
+  </si>
+  <si>
+    <t>0039281023</t>
+  </si>
+  <si>
+    <t>2 Pos Header</t>
+  </si>
+  <si>
+    <t>2 Pos Receptacle</t>
+  </si>
+  <si>
+    <t>39-01-2020</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/product-detail/en/molex-llc/39-01-2020/WM3700-ND/61315</t>
+  </si>
+  <si>
+    <t>WM3700-ND</t>
+  </si>
+  <si>
+    <t>Crimp</t>
+  </si>
+  <si>
+    <t>Mini-fit Jr Crimp</t>
+  </si>
+  <si>
+    <t>39-00-0038</t>
+  </si>
+  <si>
+    <t>WM2501CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/product-detail/en/molex-llc/39-00-0038/WM2501CT-ND/467978</t>
+  </si>
+  <si>
+    <t>Asym 4 Pin Header</t>
+  </si>
+  <si>
+    <t>WM4330-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/products/en?keywords=0470531000</t>
+  </si>
+  <si>
+    <t>WM1114-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/product-detail/en/molex-llc/08-50-0114/WM1114-ND/26475</t>
+  </si>
+  <si>
+    <t>Uni</t>
+  </si>
+  <si>
+    <t>08-50-0114</t>
+  </si>
+  <si>
+    <t>3 Pos Header</t>
+  </si>
+  <si>
+    <t>WM4201-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/product-detail/en/molex-llc/0022232031/WM4201-ND/26669</t>
+  </si>
+  <si>
+    <t>WM2012-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/product-detail/en/molex-llc/0022012037/WM2012-ND/171992</t>
+  </si>
+  <si>
+    <t>3 Pos Receptacle</t>
+  </si>
+  <si>
+    <t>WM3801-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/product-detail/en/molex-llc/0039281043/WM3801-ND/61400</t>
+  </si>
+  <si>
+    <t>4 Pos Mini-fit Header</t>
+  </si>
+  <si>
+    <t>TSM4806CSRLGCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/product-detail/en/taiwan-semiconductor-corporation/TSM4806CS-RLG/TSM4806CSRLGCT-ND/7360374</t>
+  </si>
+  <si>
+    <t>N-Channel Mosfet</t>
+  </si>
+  <si>
+    <t>TSC</t>
+  </si>
+  <si>
+    <t>TSM4806CS RLG</t>
+  </si>
+  <si>
+    <t>Mosfet Driver</t>
+  </si>
+  <si>
+    <t>Diodes Inc.</t>
+  </si>
+  <si>
+    <t>ZXGD3003E6TA</t>
+  </si>
+  <si>
+    <t>ZXGD3003E6CT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/product-detail/en/diodes-incorporated/ZXGD3003E6TA/ZXGD3003E6CT-ND/1827766</t>
+  </si>
+  <si>
+    <t>Breakout + Ribbon</t>
+  </si>
+  <si>
+    <t>RK Education</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/Raspberry-GPIO-Breakout-Ribbon-Cable/dp/B00TU3EJSW/ref=sr_1_9?s=computers&amp;ie=UTF8&amp;qid=1517494008&amp;sr=1-9&amp;keywords=raspberry%20pi%20ribbon</t>
+  </si>
+  <si>
+    <t>B00TU3EJSW</t>
+  </si>
+  <si>
+    <t>22-23-2021</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/product-detail/en/molex-llc/22-23-2021/WM4200-ND/26667</t>
+  </si>
+  <si>
+    <t>WM4200-ND</t>
+  </si>
+  <si>
+    <t>22-01-3027</t>
+  </si>
+  <si>
+    <t>WM2000-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/product-detail/en/molex-llc/22-01-3027/WM2000-ND/26431</t>
+  </si>
+  <si>
+    <t>2 Pos Header MF</t>
+  </si>
+  <si>
+    <t>2 Pos Receptacle MF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,13 +323,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -185,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -194,6 +365,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,11 +656,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J202"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +669,7 @@
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -564,7 +747,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" ref="C7:C12" si="0">A7*B7</f>
+        <f t="shared" ref="C7:C26" si="0">A7*B7</f>
         <v>8</v>
       </c>
       <c r="E7" t="s">
@@ -728,132 +911,482 @@
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I14" s="4"/>
-      <c r="J14" s="2"/>
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0.44</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.88</v>
+      </c>
+      <c r="E14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="5"/>
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.2</v>
+      </c>
       <c r="C15" s="5">
-        <f>SUM(C6:C12)</f>
-        <v>59.5</v>
-      </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="2"/>
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I16" s="4"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="4"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I18" s="4"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I19" s="4"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="4"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I21" s="4"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I22" s="4"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I23" s="4"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I24" s="4"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I25" s="4"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I26" s="4"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="8">
+        <v>470531000</v>
+      </c>
+      <c r="H17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="C18" s="5">
+        <f t="shared" si="0"/>
+        <v>1.65</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.16</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="10">
+        <v>22232031</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="8">
+        <v>22012037</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.54</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="8">
+        <v>39281043</v>
+      </c>
+      <c r="H21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.37</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" si="0"/>
+        <v>0.37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0.42</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" si="0"/>
+        <v>0.42</v>
+      </c>
+      <c r="E23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="C24" s="5">
+        <f t="shared" si="0"/>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="E24" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="C25" s="5">
+        <f t="shared" si="0"/>
+        <v>0.22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="C26" s="5">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
       <c r="I27" s="4"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5">
+        <f>SUM(C6:C26)</f>
+        <v>67.790000000000006</v>
+      </c>
       <c r="I28" s="4"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I29" s="4"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G30" s="7"/>
+      <c r="I30" s="4"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I31" s="4"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I32" s="4"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I33" s="4"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I34" s="4"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I35" s="4"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I36" s="4"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I37" s="4"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I38" s="4"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I39" s="4"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I40" s="4"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I41" s="4"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I42" s="4"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J48" s="2"/>
     </row>
     <row r="49" spans="10:10" x14ac:dyDescent="0.25">
@@ -1317,6 +1850,45 @@
     </row>
     <row r="202" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J202" s="2"/>
+    </row>
+    <row r="203" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J203" s="2"/>
+    </row>
+    <row r="204" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J204" s="2"/>
+    </row>
+    <row r="205" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J205" s="2"/>
+    </row>
+    <row r="206" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J206" s="2"/>
+    </row>
+    <row r="207" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J207" s="2"/>
+    </row>
+    <row r="208" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J208" s="2"/>
+    </row>
+    <row r="209" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J209" s="2"/>
+    </row>
+    <row r="210" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J210" s="2"/>
+    </row>
+    <row r="211" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J211" s="2"/>
+    </row>
+    <row r="212" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J212" s="2"/>
+    </row>
+    <row r="213" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J213" s="2"/>
+    </row>
+    <row r="214" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J214" s="2"/>
+    </row>
+    <row r="215" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J215" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>